<commit_message>
fix test 2 and update naming convention
</commit_message>
<xml_diff>
--- a/Q2/time_log.xlsx
+++ b/Q2/time_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdw12_000\Desktop\Ara\BCPR280_Part1\Q1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdw12_000\Desktop\Ara\BCPR280_Part1\Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4219E70-3A60-479A-9AFC-4022D3341067}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0F7FFF-1B67-44CE-9894-C472EDB45599}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10470" yWindow="945" windowWidth="18330" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5850" yWindow="1920" windowWidth="18330" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>PSP Time Recording Log</t>
   </si>
@@ -393,10 +393,6 @@
   </si>
   <si>
     <t>Starting test for code</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Found some issues and the way to fix</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -1023,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1103,13 +1099,13 @@
         <v>39</v>
       </c>
       <c r="C7" s="14">
-        <v>43543</v>
+        <v>43557</v>
       </c>
       <c r="D7" s="15">
-        <v>0.89930555555555547</v>
+        <v>0.9194444444444444</v>
       </c>
       <c r="F7" s="15">
-        <v>0.92708333333333337</v>
+        <v>0.92986111111111114</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
@@ -1120,13 +1116,13 @@
         <v>41</v>
       </c>
       <c r="C8" s="14">
-        <v>43549</v>
+        <v>43557</v>
       </c>
       <c r="D8" s="15">
-        <v>0.92291666666666661</v>
+        <v>0.92986111111111114</v>
       </c>
       <c r="F8" s="15">
-        <v>0.94930555555555562</v>
+        <v>0.95972222222222225</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -1137,13 +1133,13 @@
         <v>43</v>
       </c>
       <c r="C9" s="14">
-        <v>43549</v>
+        <v>43557</v>
       </c>
       <c r="D9" s="15">
-        <v>0.95138888888888884</v>
+        <v>0.96250000000000002</v>
       </c>
       <c r="F9" s="15">
-        <v>0.96388888888888891</v>
+        <v>0.98263888888888884</v>
       </c>
       <c r="H9" t="s">
         <v>44</v>
@@ -1154,13 +1150,13 @@
         <v>43</v>
       </c>
       <c r="C10" s="14">
-        <v>43553</v>
+        <v>43557</v>
       </c>
       <c r="D10" s="15">
-        <v>0.9819444444444444</v>
+        <v>0.98333333333333339</v>
       </c>
       <c r="F10" s="15">
-        <v>0.50902777777777775</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="H10" t="s">
         <v>45</v>
@@ -1168,70 +1164,36 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11" s="14">
         <v>43554</v>
       </c>
       <c r="D11" s="15">
-        <v>2.2916666666666669E-2</v>
+        <v>0.62430555555555556</v>
       </c>
       <c r="F11" s="15">
-        <v>4.7916666666666663E-2</v>
+        <v>0.64166666666666672</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="14">
+        <v>43556</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0.70347222222222217</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0.74583333333333324</v>
+      </c>
+      <c r="H12" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" s="14">
-        <v>43554</v>
-      </c>
-      <c r="D12" s="15">
-        <v>0.62430555555555556</v>
-      </c>
-      <c r="F12" s="15">
-        <v>0.64166666666666672</v>
-      </c>
-      <c r="H12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="14">
-        <v>43554</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.66875000000000007</v>
-      </c>
-      <c r="F13" s="15">
-        <v>0.68888888888888899</v>
-      </c>
-      <c r="H13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="14">
-        <v>43556</v>
-      </c>
-      <c r="D14" s="15">
-        <v>0.70347222222222217</v>
-      </c>
-      <c r="F14" s="15">
-        <v>0.74583333333333324</v>
-      </c>
-      <c r="H14" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>